<commit_message>
fix: TP4 Exercise 1 Factorial Excel
</commit_message>
<xml_diff>
--- a/TP4/factorial/Traza_Factorial.xlsx
+++ b/TP4/factorial/Traza_Factorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\campe\Desktop\Algoritmica-y-Programacion-2\TP4\factorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64D8AF5F-5082-4A59-A87B-CC1DE61C7F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC2FAEB-96FF-4788-9637-02315087D7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +347,23 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -431,15 +448,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -760,11 +779,15 @@
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8" ht="20.3" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1052,147 +1075,177 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="18" spans="2:11" ht="20.3" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" ht="2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:11" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="7">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="2">
         <v>2</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="7">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="2">
         <v>3</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="2">
         <v>6</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="7">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
         <v>4</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="2">
         <v>4</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="2">
         <v>24</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
         <v>5</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="2">
         <v>5</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="2">
         <v>120</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="8">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
         <v>6</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="3">
         <v>120</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="28" spans="2:11" ht="20.3" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B30:K30"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>